<commit_message>
fix xlsx autofit code; improve readme
</commit_message>
<xml_diff>
--- a/sample_excel_data.xlsx
+++ b/sample_excel_data.xlsx
@@ -1,28 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\0.SurfaceOwl\dev\xlsx_nice_column_widths\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Dropbox\0.SurfaceOwl\dev\xlsx_autofit_columns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7340F985-B258-4543-8792-819FE3C1CA17}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DDA68B-36F4-4349-9B58-6FA9E2E76334}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32880" windowHeight="17325" xr2:uid="{800EA8CF-4C9E-4FDD-B505-AA64824F2AAA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +28,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+  <si>
+    <t>column name</t>
+  </si>
   <si>
     <t>Column 1</t>
   </si>
@@ -38,19 +39,52 @@
     <t>Column 2</t>
   </si>
   <si>
-    <t>test data in row 2, column 1</t>
-  </si>
-  <si>
-    <t>short data in column 2</t>
+    <t>Column 3</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS BELOW</t>
+  </si>
+  <si>
+    <t>in excel manually change column width to match  text in this row</t>
+  </si>
+  <si>
+    <t>Colum</t>
+  </si>
+  <si>
+    <t>short data</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>longest col</t>
+  </si>
+  <si>
+    <t>keep row 2 null</t>
+  </si>
+  <si>
+    <t>data row</t>
+  </si>
+  <si>
+    <t>longest row 2, column 1</t>
   </si>
   <si>
     <t>row 3</t>
   </si>
   <si>
-    <t>Column 3</t>
-  </si>
-  <si>
-    <t>row 3 row 3 row 3</t>
+    <t>row</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>max len in col</t>
+  </si>
+  <si>
+    <t>min len in col</t>
   </si>
 </sst>
 </file>
@@ -92,11 +126,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
       </font>
       <fill>
         <patternFill>
@@ -104,21 +137,9 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{AAEC6EA4-E7EB-41FC-92A2-630D1D9DB01C}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
@@ -429,19 +450,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9157212-E974-46C4-A63C-E7799EC0C713}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="1.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,26 +473,97 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <f>MAX(LEN(D1), LEN(D5), LEN(D6), LEN(D4), LEN(D3))</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="D8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>